<commit_message>
تعديل تلقائي في شيت Card1 by admin at 2025-11-02 19:04:35
</commit_message>
<xml_diff>
--- a/bel2.xlsx
+++ b/bel2.xlsx
@@ -7456,18 +7456,66 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>م.صيام</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7500,19 +7548,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>15\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7530,18 +7610,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7559,7 +7687,11 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7575,22 +7707,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>29\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7613,29 +7769,61 @@
           <t>565</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>5\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7658,16 +7846,36 @@
           <t>724</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7678,9 +7886,21 @@
           <t>5\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7703,25 +7923,61 @@
           <t>859</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>24\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7739,18 +7995,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7768,18 +8072,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7797,18 +8149,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7826,18 +8226,66 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7951,66 +8399,18 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8028,11 +8428,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8043,51 +8439,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8105,11 +8469,7 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8125,46 +8485,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8182,66 +8514,18 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8264,61 +8548,25 @@
           <t>559</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8341,36 +8589,16 @@
           <t>727</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8381,21 +8609,9 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8418,11 +8634,7 @@
           <t>860</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8433,41 +8645,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>م.محمد عبدالله</t>
@@ -8500,36 +8688,12 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
@@ -8540,11 +8704,7 @@
           <t xml:space="preserve">تم سن فلاتس وعياره </t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t xml:space="preserve">م.محمد عبدالله </t>
@@ -8567,66 +8727,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8644,66 +8756,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8721,66 +8785,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8798,66 +8814,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
تعديل تلقائي في شيت Card2 by admin at 2025-11-02 19:07:44
</commit_message>
<xml_diff>
--- a/bel2.xlsx
+++ b/bel2.xlsx
@@ -7456,61 +7456,17 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
@@ -7548,51 +7504,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>15\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7610,66 +7534,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7687,11 +7563,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7707,46 +7579,22 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>29\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7769,61 +7617,29 @@
           <t>565</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>5\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7846,36 +7662,16 @@
           <t>724</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7886,21 +7682,9 @@
           <t>5\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7923,61 +7707,25 @@
           <t>859</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>24\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7995,66 +7743,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8072,66 +7772,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8149,66 +7801,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8226,66 +7830,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8399,18 +7955,66 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>صيام</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8428,7 +8032,11 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8439,19 +8047,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8469,7 +8109,11 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8485,18 +8129,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8514,18 +8186,66 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8548,25 +8268,61 @@
           <t>559</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8589,16 +8345,36 @@
           <t>727</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8609,9 +8385,21 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8634,7 +8422,11 @@
           <t>860</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8645,17 +8437,41 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O8" t="inlineStr">
         <is>
           <t>م.محمد عبدالله</t>
@@ -8688,12 +8504,36 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
@@ -8704,7 +8544,11 @@
           <t xml:space="preserve">تم سن فلاتس وعياره </t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O9" t="inlineStr">
         <is>
           <t xml:space="preserve">م.محمد عبدالله </t>
@@ -8727,18 +8571,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8756,18 +8648,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8785,18 +8725,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8814,18 +8802,66 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
تعديل تلقائي في شيت Card24 by admin at 2025-11-02 19:11:18
</commit_message>
<xml_diff>
--- a/bel2.xlsx
+++ b/bel2.xlsx
@@ -556,20 +556,56 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
@@ -592,18 +628,66 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -621,18 +705,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -650,18 +782,66 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -684,7 +864,11 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -705,16 +889,36 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -737,7 +941,11 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -748,18 +956,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -777,18 +1013,66 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -806,18 +1090,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -835,18 +1167,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -864,18 +1244,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -893,18 +1321,66 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7955,61 +8431,17 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>صيام</t>
@@ -8032,11 +8464,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8047,51 +8475,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8109,11 +8505,7 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8129,46 +8521,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8186,66 +8550,18 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8268,61 +8584,25 @@
           <t>559</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8345,36 +8625,16 @@
           <t>727</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8385,21 +8645,9 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8422,11 +8670,7 @@
           <t>860</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8437,41 +8681,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>م.محمد عبدالله</t>
@@ -8504,36 +8724,12 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
@@ -8544,11 +8740,7 @@
           <t xml:space="preserve">تم سن فلاتس وعياره </t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t xml:space="preserve">م.محمد عبدالله </t>
@@ -8571,66 +8763,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8648,66 +8792,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8725,66 +8821,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8802,66 +8850,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
إضافة عمود Current Tons لجميع الكروت by admin at 2025-11-11 18:55:14
</commit_message>
<xml_diff>
--- a/bel2.xlsx
+++ b/bel2.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,6 +530,11 @@
       <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Serviced by</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
         </is>
       </c>
     </row>
@@ -561,6 +566,9 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -590,6 +598,9 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -619,6 +630,9 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -648,6 +662,9 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -677,6 +694,9 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -706,6 +726,9 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -735,6 +758,9 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -764,6 +790,9 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -793,6 +822,9 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -822,6 +854,9 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -851,6 +886,9 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -863,7 +901,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -932,6 +970,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -952,6 +995,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -972,6 +1018,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -992,6 +1041,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1012,6 +1064,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1032,6 +1087,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1052,6 +1110,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1072,6 +1133,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1092,6 +1156,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1112,6 +1179,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1132,6 +1202,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1152,6 +1225,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1164,7 +1240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1233,6 +1309,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1253,6 +1334,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1273,6 +1357,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1293,6 +1380,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1313,6 +1403,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1333,6 +1426,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1353,6 +1449,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1373,6 +1472,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1393,6 +1495,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1413,6 +1518,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1433,6 +1541,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1453,6 +1564,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1465,7 +1579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1534,6 +1648,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1554,6 +1673,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1574,6 +1696,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1594,6 +1719,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1614,6 +1742,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1634,6 +1765,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1654,6 +1788,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1674,6 +1811,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1694,6 +1834,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1714,6 +1857,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1734,6 +1880,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1754,6 +1903,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1766,7 +1918,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1835,6 +1987,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1855,6 +2012,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1875,6 +2035,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1895,6 +2058,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1915,6 +2081,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1935,6 +2104,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1955,6 +2127,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1975,6 +2150,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1995,6 +2173,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -2015,6 +2196,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -2035,6 +2219,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -2055,6 +2242,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2067,7 +2257,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2136,6 +2326,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -2156,6 +2351,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -2176,6 +2374,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -2196,6 +2397,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -2216,6 +2420,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -2236,6 +2443,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -2256,6 +2466,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -2276,6 +2489,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -2296,6 +2512,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -2316,6 +2535,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -2336,6 +2558,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -2356,6 +2581,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2368,7 +2596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2437,6 +2665,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -2457,6 +2690,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -2477,6 +2713,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -2497,6 +2736,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -2517,6 +2759,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -2537,6 +2782,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -2557,6 +2805,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -2577,6 +2828,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -2597,6 +2851,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -2617,6 +2874,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -2637,6 +2897,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -2657,6 +2920,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2669,7 +2935,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2751,6 +3017,11 @@
       <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Serviced by</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
         </is>
       </c>
     </row>
@@ -2782,6 +3053,9 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2811,6 +3085,9 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2840,6 +3117,9 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2869,6 +3149,9 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2898,6 +3181,9 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2927,6 +3213,9 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2956,6 +3245,9 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2985,6 +3277,9 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3014,6 +3309,9 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3043,6 +3341,9 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3072,6 +3373,9 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3084,7 +3388,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3153,6 +3457,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -3173,6 +3482,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -3193,6 +3505,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -3213,6 +3528,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -3233,6 +3551,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -3253,6 +3574,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -3273,6 +3597,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -3293,6 +3620,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -3313,6 +3643,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -3333,6 +3666,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -3353,6 +3689,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -3373,6 +3712,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3385,7 +3727,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3454,6 +3796,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -3474,6 +3821,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -3494,6 +3844,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -3514,6 +3867,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -3534,6 +3890,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -3554,6 +3913,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -3574,6 +3936,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -3594,6 +3959,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -3614,6 +3982,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -3634,6 +4005,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -3654,6 +4028,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -3674,6 +4051,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3686,7 +4066,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3755,6 +4135,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -3775,6 +4160,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -3797,6 +4185,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -3817,6 +4208,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -3837,6 +4231,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -3859,6 +4256,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -3881,6 +4281,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -3903,6 +4306,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -3923,6 +4329,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -3943,6 +4352,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -3963,6 +4375,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -3983,6 +4398,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3995,7 +4413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4077,6 +4495,11 @@
       <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Serviced by</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
         </is>
       </c>
     </row>
@@ -4102,6 +4525,9 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -4125,6 +4551,9 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -4148,6 +4577,9 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -4171,6 +4603,9 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -4194,6 +4629,9 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -4217,6 +4655,9 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -4240,6 +4681,9 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -4263,6 +4707,9 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -4286,6 +4733,9 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -4309,6 +4759,9 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -4332,6 +4785,9 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4344,7 +4800,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4413,6 +4869,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -4433,6 +4894,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -4453,6 +4917,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -4473,6 +4940,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -4493,6 +4963,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -4513,6 +4986,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -4533,6 +5009,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -4553,6 +5032,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -4573,6 +5055,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -4593,6 +5078,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -4613,6 +5101,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -4633,6 +5124,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5805,7 +6299,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5889,954 +6383,16 @@
           <t>Serviced by</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">done </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>م.صيام</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>card</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Min_Tones</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Max_Tones</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Tones</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(x)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>1.carding elemnt(o)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>licker_in carding element(o)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Doffer carding element(o)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>cylinder(X)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>doffer(X)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(o)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Correction</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Serviced by</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -6861,6 +6417,478 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">done </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>م.صيام</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>card</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Min_Tones</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Max_Tones</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tones</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(x)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>1.carding elemnt(o)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>licker_in carding element(o)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Doffer carding element(o)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>cylinder(X)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>doffer(X)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(o)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -6890,6 +6918,9 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -6919,6 +6950,9 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -6948,6 +6982,9 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -6977,6 +7014,9 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7006,6 +7046,9 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7035,6 +7078,9 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7064,6 +7110,9 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7093,6 +7142,9 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7122,6 +7174,9 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7151,6 +7206,9 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -7180,6 +7238,9 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7192,7 +7253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7274,6 +7335,11 @@
       <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Serviced by</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
         </is>
       </c>
     </row>
@@ -7299,6 +7365,9 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -7322,6 +7391,9 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -7345,6 +7417,9 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -7368,6 +7443,9 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -7391,6 +7469,9 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -7414,6 +7495,9 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -7437,6 +7521,9 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -7460,6 +7547,9 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -7483,6 +7573,9 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -7506,6 +7599,9 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -7529,6 +7625,9 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7541,7 +7640,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7610,6 +7709,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -7630,6 +7734,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -7650,6 +7757,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -7670,6 +7780,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -7690,6 +7803,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -7710,6 +7826,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -7730,6 +7849,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -7750,6 +7872,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -7770,6 +7895,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -7790,6 +7918,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -7810,6 +7941,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -7830,6 +7964,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7842,7 +7979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7911,6 +8048,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7937,6 +8079,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7963,6 +8108,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7989,6 +8137,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8015,6 +8166,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8041,6 +8195,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8067,6 +8224,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8093,6 +8253,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8119,6 +8282,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8145,6 +8311,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8171,6 +8340,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8197,6 +8369,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8209,7 +8384,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8278,6 +8453,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -8298,6 +8478,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -8318,6 +8501,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -8338,6 +8524,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -8358,6 +8547,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -8378,6 +8570,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -8398,6 +8593,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -8418,6 +8616,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -8438,6 +8639,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -8458,6 +8662,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -8478,6 +8685,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -8498,6 +8708,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8510,7 +8723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8579,6 +8792,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -8599,6 +8817,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -8619,6 +8840,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -8639,6 +8863,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -8659,6 +8886,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -8679,6 +8909,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -8699,6 +8932,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -8719,6 +8955,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -8739,6 +8978,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -8759,6 +9001,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -8779,6 +9024,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -8799,6 +9047,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8811,7 +9062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8893,6 +9144,11 @@
       <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Serviced by</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
         </is>
       </c>
     </row>
@@ -8924,6 +9180,9 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8953,6 +9212,9 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8982,6 +9244,9 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9011,6 +9276,9 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9040,6 +9308,9 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9069,6 +9340,9 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9098,6 +9372,9 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -9127,6 +9404,9 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -9156,6 +9436,9 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -9185,6 +9468,9 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -9214,6 +9500,9 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9226,7 +9515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9295,6 +9584,11 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Current Tons</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -9315,6 +9609,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -9335,6 +9632,9 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -9355,6 +9655,9 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -9375,6 +9678,9 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -9395,6 +9701,9 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -9415,6 +9724,9 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -9435,6 +9747,9 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -9455,6 +9770,9 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -9475,6 +9793,9 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -9495,6 +9816,9 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -9515,6 +9839,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
تحديث إنتاج Card1: 2070.00 طن → 2070.00 طن by admin at 2025-11-11 18:56:53
</commit_message>
<xml_diff>
--- a/bel2.xlsx
+++ b/bel2.xlsx
@@ -6299,7 +6299,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6755,6 +6755,26 @@
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="n">
+        <v>2070</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
تحديث إنتاج Card1: 941.87 طن → 3011.87 طن by admin at 2025-11-11 19:53:56
</commit_message>
<xml_diff>
--- a/bel2.xlsx
+++ b/bel2.xlsx
@@ -6299,7 +6299,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6775,6 +6775,26 @@
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
         <v>2070</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>3011.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>